<commit_message>
SC QCADOOCLS-7576 Added additional unit and conversion column to products import.
</commit_message>
<xml_diff>
--- a/mes-plugins/mes-plugins-basic/src/main/resources/basic/public/resources/productImportSchema_pl.xlsx
+++ b/mes-plugins/mes-plugins-basic/src/main/resources/basic/public/resources/productImportSchema_pl.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28810"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/monikajedrysiak/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lupo/qcadoo-src/mes/mes-plugins/mes-plugins-basic/src/main/resources/basic/public/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09E460C-43AC-CE4E-96B2-72A3460C7C2E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="9740" windowWidth="33600" windowHeight="9400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,13 +31,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
-    <author>qcadoo MES</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -84,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -114,113 +114,161 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">- surowiec
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">- półprodukt
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">- finalny produkt
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>- odpad</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">qcadoo MES:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Dana wymagana. Użyj wartości jednostki zdefiniowanej w słowniku</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">qcadoo MES:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Dana opcjonalna. Jeśli chcesz podać EANy dla produktów, pamiętaj, że dany kod może być przypisany tylko do 1 produktu</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">qcadoo MES:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Dana opcjonalna. Jeśli chcesz przypisz produkt do kategorii, wpisując wartość ze słownika kategorii</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0">
+          <t xml:space="preserve">- surowiec,
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- półprodukt,
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- finalny produkt,
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>- odpad.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">qcadoo MES:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dana wymagana. Użyj wartości jednostki zdefiniowanej w słowniku.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{5830D5F2-87E2-844B-8797-8AC985758524}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">qcadoo MES:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dana opcjonalna. Wskaż jednostkę, z listy zdefiniowanej w słowniku, w której chcesz dodatkowo prowadzić ewidencję magazynową. Podana jednostka musi być różna niż jednostka podstawowa. Pamiętaj o podaniu w następnej kolumnie przelicznika między jednostkami.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{3B4D0B4C-397E-C54A-802C-74C233498F1A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">qcadoo MES:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Dana wymagana, gdy produkt ma jednostkę dodatkową. Podaj ile jednostek dodatkowych mieści się w jednej jednostce podstawowej produktu. Przykład: jednostka podstawowa to karton, jednostka dodatkowa do sztuka. Jeśli w kartonie mamy 10 sztuk produktu, to przelicznik = 10.  </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">qcadoo MES:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dana opcjonalna. Jeśli chcesz podać EANy dla produktów, pamiętaj, że dany kod może być przypisany tylko do 1 produktu.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">qcadoo MES:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dana opcjonalna. Jeśli chcesz przypisz produkt do kategorii, wpisując wartość ze słownika kategorii.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -244,79 +292,79 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">qcadoo MES:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Dana opcjonalna. Jeśli chcesz określić producenta produktu użyj numeru klienta zdefiniowanego w qcadoo</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">qcadoo MES:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Dana opcjolana. Jeśli chcesz przypisać produkt do asortymentu, użyj nazwy asortymentu zdefiniowanego w qcadoo</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">qcadoo MES:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Dana opcjonalna. Możesz przypisać produkt do rodziny - w tym celu zdefiniuj w qcadoo produkty - rodziny i użyj w pliku importu ich numeru</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">qcadoo MES:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dana opcjonalna. Jeśli chcesz określić producenta produktu użyj numeru klienta zdefiniowanego w qcadoo.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">qcadoo MES:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dana opcjolana. Jeśli chcesz przypisać produkt do asortymentu, użyj nazwy asortymentu zdefiniowanego w qcadoo.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">qcadoo MES:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dana opcjonalna. Możesz przypisać produkt do rodziny - w tym celu zdefiniuj w qcadoo produkty - rodziny i użyj w pliku importu ich numeru.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -340,7 +388,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -364,7 +412,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -388,75 +436,75 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>qcadoo MES:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Dana opcjonalna.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O1" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>qcadoo MES:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Dana opcjonalna. Ważność wyrażana jest w miesiacach. Podana wartość musi być liczbą dodatnią całkowitą.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P1" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>qcadoo MES:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Dana opcjonalna.  Dostępne wartości: 'tak' lub 'nie'. Jeśli komórka będzie pusta lub wartość będzie inna niż dostępne, to ewidencja partii nie będzie wymagana.</t>
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{FF493189-EE86-DB48-BBD1-C407EC7EAA15}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">qcadoo MES:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dana opcjonalna</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{E2643E46-76DC-BC41-853C-2A72829A86F0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">qcadoo MES:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dana opcjonalna. Ważność wyrażana jest w miesiacach. Podana wartość musi być liczbą dodatnią całkowitą.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{12BA27A3-B592-B941-BFB3-4A02442816BD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">qcadoo MES:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dana opcjonalna.  Dostępne wartości: 'tak' lub 'nie'. Jeśli komórka będzie pusta lub wartość będzie inna niż dostępne, to ewidencja partii nie będzie wymagana.</t>
         </r>
       </text>
     </comment>
@@ -465,7 +513,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Numer</t>
   </si>
@@ -513,13 +561,19 @@
   </si>
   <si>
     <t>Ewidencja partii</t>
+  </si>
+  <si>
+    <t>Przelicznik</t>
+  </si>
+  <si>
+    <t>jednostka dodatkowa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -545,19 +599,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="81"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -591,13 +632,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Norm." xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -622,7 +662,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1117600</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -632,7 +672,7 @@
         <xdr:cNvPr id="1050" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E97A3254-EBA0-0A45-BB7C-63DAE4259A85}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E97A3254-EBA0-0A45-BB7C-63DAE4259A85}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -671,7 +711,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1117600</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -681,7 +721,7 @@
         <xdr:cNvPr id="1048" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3324B8BE-F0F9-D04D-B919-178894C1FEE4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3324B8BE-F0F9-D04D-B919-178894C1FEE4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -720,7 +760,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1117600</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -730,7 +770,7 @@
         <xdr:cNvPr id="1046" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72EB3432-E52C-E341-8116-3225AC86D3E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72EB3432-E52C-E341-8116-3225AC86D3E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -769,7 +809,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1117600</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -779,7 +819,7 @@
         <xdr:cNvPr id="1044" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F131412A-160F-E64F-967F-F09418532A3C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F131412A-160F-E64F-967F-F09418532A3C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -818,7 +858,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1117600</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -828,7 +868,7 @@
         <xdr:cNvPr id="1042" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39FF3EAF-68FD-9346-813A-9FE8937BB301}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39FF3EAF-68FD-9346-813A-9FE8937BB301}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -867,7 +907,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1117600</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -877,7 +917,7 @@
         <xdr:cNvPr id="1040" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A9E0793-ECA4-F341-A219-451E356AFEAB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A9E0793-ECA4-F341-A219-451E356AFEAB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -916,7 +956,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1117600</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -926,7 +966,7 @@
         <xdr:cNvPr id="1038" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61D3C515-0182-0C44-8CF1-5B09D4BC5EF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61D3C515-0182-0C44-8CF1-5B09D4BC5EF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -965,7 +1005,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1117600</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -975,7 +1015,7 @@
         <xdr:cNvPr id="1036" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5E7E608-94EB-4543-94BE-BF3E0B7910AB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5E7E608-94EB-4543-94BE-BF3E0B7910AB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1014,7 +1054,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1117600</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -1024,7 +1064,7 @@
         <xdr:cNvPr id="1034" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30786922-EB01-134F-BCB4-70E2DC99309B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30786922-EB01-134F-BCB4-70E2DC99309B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1063,7 +1103,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1117600</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -1073,7 +1113,7 @@
         <xdr:cNvPr id="1032" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15D1A257-F1D4-8E4B-A30F-ABA7BC329DA8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15D1A257-F1D4-8E4B-A30F-ABA7BC329DA8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1112,7 +1152,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1117600</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -1122,7 +1162,7 @@
         <xdr:cNvPr id="1030" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7485639-714A-4747-AD3E-5B7C923BB237}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7485639-714A-4747-AD3E-5B7C923BB237}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1161,7 +1201,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1117600</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -1171,7 +1211,7 @@
         <xdr:cNvPr id="1028" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02CC3FAB-C0BF-A747-A87B-8E61A4DE4DB2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02CC3FAB-C0BF-A747-A87B-8E61A4DE4DB2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1210,7 +1250,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1117600</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -1220,7 +1260,7 @@
         <xdr:cNvPr id="1026" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B7B3336-3A71-4546-86DD-F4C78B874A40}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B7B3336-3A71-4546-86DD-F4C78B874A40}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1550,23 +1590,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="4" width="20.83203125" customWidth="1"/>
-    <col min="5" max="10" width="16.83203125" customWidth="1"/>
-    <col min="11" max="13" width="20.83203125" customWidth="1"/>
-    <col min="16" max="16" width="15.83203125" customWidth="1"/>
+    <col min="3" max="5" width="20.83203125" customWidth="1"/>
+    <col min="6" max="12" width="16.83203125" customWidth="1"/>
+    <col min="13" max="15" width="20.83203125" customWidth="1"/>
+    <col min="16" max="18" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1580,39 +1620,45 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>